<commit_message>
fix broken requires when run from gem
</commit_message>
<xml_diff>
--- a/spec/fixtures/ProjectsSingleCategories.xlsx
+++ b/spec/fixtures/ProjectsSingleCategories.xlsx
@@ -94,6 +94,7 @@
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -115,6 +116,7 @@
       <sz val="10"/>
       <name val="Verdana"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -236,6 +238,7 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.75"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.8705357142857"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="28.1919642857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.79017857142857"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -329,7 +332,7 @@
       </c>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>

</xml_diff>